<commit_message>
inventory update and april tags
</commit_message>
<xml_diff>
--- a/NU-Smarticle PCB Design/BOMs/Inventory-v2.0.xlsx
+++ b/NU-Smarticle PCB Design/BOMs/Inventory-v2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsamland/Documents/GitHub/NU-Smarticle/NU-Smarticle PCB Design/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC392860-4C88-0646-BCEF-E8640476AFD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71DBC65-CE42-5842-B64D-82F95DB03369}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{D63DB3F0-E8B1-1F4E-9AB0-B5BC2EC9A6FA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{D63DB3F0-E8B1-1F4E-9AB0-B5BC2EC9A6FA}"/>
   </bookViews>
   <sheets>
     <sheet name="TopBoard" sheetId="5" r:id="rId1"/>
@@ -671,9 +671,6 @@
     <t>Op Amp</t>
   </si>
   <si>
-    <t>qty as of 10/11/19</t>
-  </si>
-  <si>
     <t>Feathers Made</t>
   </si>
   <si>
@@ -705,6 +702,9 @@
   </si>
   <si>
     <t>HobbyKing</t>
+  </si>
+  <si>
+    <t>qty as of 12/11/19</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
     <font>
       <i/>
       <sz val="12"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -842,7 +842,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1170,7 +1170,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection sqref="A1:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,6 +1433,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1440,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC9AD7B-F263-A14F-B1B2-5A8DBADE0C7E}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="92" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2748,8 +2749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858D28EE-AF03-6F46-82F7-ED1679C381D3}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2773,31 +2774,31 @@
         <v>81</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>201</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2809,13 +2810,13 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I2" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="7"/>
     </row>
@@ -2852,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2867,7 +2868,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -2882,7 +2883,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2912,7 +2913,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="5">
-        <v>940</v>
+        <v>917</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2942,7 +2943,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="4">
-        <v>460</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -2972,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="4">
-        <v>450</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -3008,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -3038,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="4">
-        <v>940</v>
+        <v>924</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3068,7 +3069,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="4">
-        <v>930</v>
+        <v>909</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -3098,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="4">
-        <v>960</v>
+        <v>948</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -3115,14 +3116,14 @@
         <v>129</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E17">
         <f>K17-G17-$H$2*H17-I$2*I17-J$2*J17+F17</f>
         <v>6</v>
       </c>
       <c r="F17" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G17" s="6">
         <v>0</v>
@@ -3137,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -3174,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -3236,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -3248,14 +3249,14 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="F23" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
@@ -3270,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -3307,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -3341,7 +3342,7 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -3375,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -3390,10 +3391,10 @@
       </c>
       <c r="E29">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G29" s="6">
         <v>2</v>
@@ -3408,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -3419,11 +3420,11 @@
         <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E30">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F30" s="6">
         <v>0</v>
@@ -3441,7 +3442,7 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -3457,7 +3458,7 @@
       </c>
       <c r="E31">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F31" s="6">
         <v>0</v>
@@ -3475,7 +3476,7 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -3508,7 +3509,7 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -3546,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -3568,23 +3569,23 @@
         <f>K38-G38-$H$2*H38-I$2*I38-J$2*J38+F38</f>
         <v>15</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="6">
+        <v>0</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
         <v>15</v>
-      </c>
-      <c r="G38" s="6">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
-      <c r="I38">
-        <v>1</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -3602,7 +3603,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G39" s="6">
         <v>0</v>
@@ -3617,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -3637,7 +3638,7 @@
       </c>
       <c r="E42">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F42" s="6">
         <v>0</v>
@@ -3655,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="K42">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -3673,7 +3674,7 @@
         <v>7</v>
       </c>
       <c r="F43" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G43" s="6">
         <v>0</v>
@@ -3688,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="K43">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -3700,10 +3701,10 @@
       </c>
       <c r="E44">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F44" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G44" s="6">
         <v>0</v>
@@ -3718,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="K44">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -3753,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="K47">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -3761,14 +3762,14 @@
         <v>188</v>
       </c>
       <c r="C48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D48" t="s">
         <v>189</v>
       </c>
       <c r="E48">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F48" s="6">
         <v>0</v>
@@ -3785,8 +3786,8 @@
       <c r="J48">
         <v>2</v>
       </c>
-      <c r="K48">
-        <v>8</v>
+      <c r="K48" s="10">
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -3794,14 +3795,14 @@
         <v>191</v>
       </c>
       <c r="C49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D49" t="s">
         <v>192</v>
       </c>
       <c r="E49">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F49" s="6">
         <v>0</v>
@@ -3819,7 +3820,7 @@
         <v>1</v>
       </c>
       <c r="K49">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>